<commit_message>
update README and filenames
</commit_message>
<xml_diff>
--- a/filter.xlsx
+++ b/filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cx\projects\hk-slope-kml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A235A7B-ECFE-4C35-BF98-8E78C4CAFABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A30009-60DB-4C20-B72E-67B756818CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Shape Fill</t>
-  </si>
-  <si>
-    <t>3. Save this workbook and run 'generate.exe'. Output will be 'ouptut.kml'.</t>
   </si>
   <si>
     <r>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>KIL 6427</t>
+  </si>
+  <si>
+    <t>3. Save this workbook and run 'generate.exe'. Output will be 'output.kml'.</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -682,7 +682,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -707,7 +707,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -718,7 +718,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="9"/>
       <c r="L5" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
@@ -754,7 +754,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="3">
         <v>2</v>
@@ -765,7 +765,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="11"/>
       <c r="L7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -790,7 +790,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="12"/>
       <c r="L8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
@@ -804,13 +804,13 @@
         <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -824,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -841,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="3">
         <v>2</v>
@@ -858,7 +858,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
@@ -875,7 +875,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="3">
         <v>3</v>
@@ -892,7 +892,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3">
         <v>3</v>
@@ -909,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="3">
         <v>3</v>
@@ -926,7 +926,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="3">
         <v>4</v>
@@ -943,7 +943,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="3">
         <v>4</v>
@@ -960,7 +960,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
@@ -971,13 +971,13 @@
         <v>123</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="3">
         <v>4</v>
@@ -988,13 +988,13 @@
         <v>125</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="3">
         <v>3</v>
@@ -1005,13 +1005,13 @@
         <v>127</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="3">
         <v>3</v>
@@ -1022,13 +1022,13 @@
         <v>129</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="3">
         <v>3</v>
@@ -1039,13 +1039,13 @@
         <v>131</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="3">
         <v>4</v>
@@ -1056,13 +1056,13 @@
         <v>133</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -1073,13 +1073,13 @@
         <v>135</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="3">
         <v>3</v>
@@ -1090,13 +1090,13 @@
         <v>137</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="3">
         <v>2</v>
@@ -1107,13 +1107,13 @@
         <v>139</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
upgrade to v0.3.1, migrate to pipenv
</commit_message>
<xml_diff>
--- a/filter.xlsx
+++ b/filter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cx\projects\hk-slope-kml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cx\projects\hk-geocoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A30009-60DB-4C20-B72E-67B756818CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87004ADB-3939-48D1-B3CE-328E014650C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t>3SE-D/C 61</t>
   </si>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1095,9 +1095,6 @@
       <c r="D26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="F26" s="3">
         <v>2</v>
       </c>
@@ -1111,9 +1108,6 @@
       </c>
       <c r="D27" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="F27" s="3">
         <v>2</v>

</xml_diff>